<commit_message>
Minor - Updating output
We realized that the Git Ignore on the pdf and the png formats was not working properly. Now we fix it.
</commit_message>
<xml_diff>
--- a/Output/5_Phospho.xlsx
+++ b/Output/5_Phospho.xlsx
@@ -1368,7 +1368,7 @@
         <v>51</v>
       </c>
       <c r="U5">
-        <v>72.71333327596909</v>
+        <v>72.71333327596911</v>
       </c>
       <c r="V5">
         <v>44.87</v>
@@ -1880,7 +1880,7 @@
         <v>51</v>
       </c>
       <c r="U9">
-        <v>40.32717350521771</v>
+        <v>40.3271735052177</v>
       </c>
       <c r="V9">
         <v>118.1</v>
@@ -1975,13 +1975,13 @@
         <v>10.25816666666667</v>
       </c>
       <c r="J10">
-        <v>7108.573909999999</v>
+        <v>7108.57391</v>
       </c>
       <c r="K10">
-        <v>78.97820499999943</v>
+        <v>78.97820500000034</v>
       </c>
       <c r="L10">
-        <v>78.97820499999943</v>
+        <v>78.97820500000034</v>
       </c>
       <c r="M10" t="s">
         <v>56</v>
@@ -2776,7 +2776,7 @@
         <v>51</v>
       </c>
       <c r="U16">
-        <v>48.80896057376221</v>
+        <v>48.8089605737622</v>
       </c>
       <c r="V16">
         <v>110.43</v>
@@ -3160,7 +3160,7 @@
         <v>51</v>
       </c>
       <c r="U19">
-        <v>41.41343162217429</v>
+        <v>41.4134316221743</v>
       </c>
       <c r="V19">
         <v>110.92</v>
@@ -3383,13 +3383,13 @@
         <v>10.854</v>
       </c>
       <c r="J21">
-        <v>7109.555340000001</v>
+        <v>7109.55534</v>
       </c>
       <c r="K21">
-        <v>79.95963500000107</v>
+        <v>79.95963500000016</v>
       </c>
       <c r="L21">
-        <v>79.95963500000107</v>
+        <v>79.95963500000016</v>
       </c>
       <c r="M21" t="s">
         <v>56</v>
@@ -3511,13 +3511,13 @@
         <v>8.565833333333334</v>
       </c>
       <c r="J22">
-        <v>7109.558379999999</v>
+        <v>7109.55838</v>
       </c>
       <c r="K22">
-        <v>79.96267499999976</v>
+        <v>79.96267500000067</v>
       </c>
       <c r="L22">
-        <v>79.96267499999976</v>
+        <v>79.96267500000067</v>
       </c>
       <c r="M22" t="s">
         <v>56</v>
@@ -3639,13 +3639,13 @@
         <v>6.59</v>
       </c>
       <c r="J23">
-        <v>7109.562120000001</v>
+        <v>7109.56212</v>
       </c>
       <c r="K23">
-        <v>79.96641500000078</v>
+        <v>79.96641499999987</v>
       </c>
       <c r="L23">
-        <v>79.96641500000078</v>
+        <v>79.96641499999987</v>
       </c>
       <c r="M23" t="s">
         <v>56</v>
@@ -3898,10 +3898,10 @@
         <v>7109.56277</v>
       </c>
       <c r="K25">
-        <v>79.96706500000073</v>
+        <v>79.96706499999982</v>
       </c>
       <c r="L25">
-        <v>79.96706500000073</v>
+        <v>79.96706499999982</v>
       </c>
       <c r="M25" t="s">
         <v>56</v>
@@ -4151,13 +4151,13 @@
         <v>11.17716666666667</v>
       </c>
       <c r="J27">
-        <v>7109.564740000001</v>
+        <v>7109.56474</v>
       </c>
       <c r="K27">
-        <v>79.96903500000099</v>
+        <v>79.96903500000008</v>
       </c>
       <c r="L27">
-        <v>79.96903500000099</v>
+        <v>79.96903500000008</v>
       </c>
       <c r="M27" t="s">
         <v>56</v>
@@ -4279,13 +4279,13 @@
         <v>9.471333333333332</v>
       </c>
       <c r="J28">
-        <v>7109.565140000001</v>
+        <v>7109.56514</v>
       </c>
       <c r="K28">
-        <v>79.96943500000089</v>
+        <v>79.96943499999998</v>
       </c>
       <c r="L28">
-        <v>79.96943500000089</v>
+        <v>79.96943499999998</v>
       </c>
       <c r="M28" t="s">
         <v>56</v>
@@ -4407,13 +4407,13 @@
         <v>13.51716666666667</v>
       </c>
       <c r="J29">
-        <v>7109.565540000001</v>
+        <v>7109.56554</v>
       </c>
       <c r="K29">
-        <v>79.96983500000078</v>
+        <v>79.96983499999988</v>
       </c>
       <c r="L29">
-        <v>79.96983500000078</v>
+        <v>79.96983499999988</v>
       </c>
       <c r="M29" t="s">
         <v>56</v>
@@ -4663,13 +4663,13 @@
         <v>11.76366666666667</v>
       </c>
       <c r="J31">
-        <v>7109.565959999999</v>
+        <v>7109.56596</v>
       </c>
       <c r="K31">
-        <v>79.97025499999927</v>
+        <v>79.97025500000018</v>
       </c>
       <c r="L31">
-        <v>79.97025499999927</v>
+        <v>79.97025500000018</v>
       </c>
       <c r="M31" t="s">
         <v>56</v>
@@ -5175,13 +5175,13 @@
         <v>4.0795</v>
       </c>
       <c r="J35">
-        <v>7109.571459999999</v>
+        <v>7109.57146</v>
       </c>
       <c r="K35">
-        <v>79.97575499999948</v>
+        <v>79.97575500000039</v>
       </c>
       <c r="L35">
-        <v>79.97575499999948</v>
+        <v>79.97575500000039</v>
       </c>
       <c r="M35" t="s">
         <v>56</v>
@@ -5303,13 +5303,13 @@
         <v>8.449333333333334</v>
       </c>
       <c r="J36">
-        <v>7109.575159999999</v>
+        <v>7109.57516</v>
       </c>
       <c r="K36">
-        <v>79.97945499999969</v>
+        <v>79.9794550000006</v>
       </c>
       <c r="L36">
-        <v>79.97945499999969</v>
+        <v>79.9794550000006</v>
       </c>
       <c r="M36" t="s">
         <v>56</v>
@@ -5687,13 +5687,13 @@
         <v>9.359500000000001</v>
       </c>
       <c r="J39">
-        <v>7109.577490000001</v>
+        <v>7109.57749</v>
       </c>
       <c r="K39">
-        <v>79.98178500000085</v>
+        <v>79.98178499999995</v>
       </c>
       <c r="L39">
-        <v>79.98178500000085</v>
+        <v>79.98178499999995</v>
       </c>
       <c r="M39" t="s">
         <v>56</v>
@@ -5943,13 +5943,13 @@
         <v>12.4265</v>
       </c>
       <c r="J41">
-        <v>7109.578420000001</v>
+        <v>7109.57842</v>
       </c>
       <c r="K41">
-        <v>79.98271500000101</v>
+        <v>79.9827150000001</v>
       </c>
       <c r="L41">
-        <v>79.98271500000101</v>
+        <v>79.9827150000001</v>
       </c>
       <c r="M41" t="s">
         <v>56</v>
@@ -6071,13 +6071,13 @@
         <v>10.25016666666667</v>
       </c>
       <c r="J42">
-        <v>7109.579659999999</v>
+        <v>7109.57966</v>
       </c>
       <c r="K42">
-        <v>79.9839549999997</v>
+        <v>79.98395500000061</v>
       </c>
       <c r="L42">
-        <v>79.9839549999997</v>
+        <v>79.98395500000061</v>
       </c>
       <c r="M42" t="s">
         <v>56</v>
@@ -7223,13 +7223,13 @@
         <v>11.14516666666667</v>
       </c>
       <c r="J51">
-        <v>7109.585120000001</v>
+        <v>7109.58512</v>
       </c>
       <c r="K51">
-        <v>79.98941500000092</v>
+        <v>79.98941500000001</v>
       </c>
       <c r="L51">
-        <v>79.98941500000092</v>
+        <v>79.98941500000001</v>
       </c>
       <c r="M51" t="s">
         <v>56</v>
@@ -7351,13 +7351,13 @@
         <v>10.08283333333333</v>
       </c>
       <c r="J52">
-        <v>7109.586270000001</v>
+        <v>7109.58627</v>
       </c>
       <c r="K52">
-        <v>79.99056500000097</v>
+        <v>79.99056500000006</v>
       </c>
       <c r="L52">
-        <v>79.99056500000097</v>
+        <v>79.99056500000006</v>
       </c>
       <c r="M52" t="s">
         <v>56</v>
@@ -7479,13 +7479,13 @@
         <v>21.382</v>
       </c>
       <c r="J53">
-        <v>7109.586429999999</v>
+        <v>7109.58643</v>
       </c>
       <c r="K53">
-        <v>79.99072499999966</v>
+        <v>79.99072500000057</v>
       </c>
       <c r="L53">
-        <v>79.99072499999966</v>
+        <v>79.99072500000057</v>
       </c>
       <c r="M53" t="s">
         <v>56</v>
@@ -7896,7 +7896,7 @@
         <v>51</v>
       </c>
       <c r="U56">
-        <v>72.71333327596909</v>
+        <v>72.71333327596911</v>
       </c>
       <c r="V56">
         <v>44.87</v>
@@ -8250,10 +8250,10 @@
         <v>13275.77464</v>
       </c>
       <c r="K59">
-        <v>78.95472699999664</v>
+        <v>78.95472699999482</v>
       </c>
       <c r="L59">
-        <v>78.95472699999664</v>
+        <v>78.95472699999482</v>
       </c>
       <c r="M59" t="s">
         <v>57</v>
@@ -8378,10 +8378,10 @@
         <v>13275.80008</v>
       </c>
       <c r="K60">
-        <v>78.98016699999425</v>
+        <v>78.98016699999607</v>
       </c>
       <c r="L60">
-        <v>78.98016699999425</v>
+        <v>78.98016699999607</v>
       </c>
       <c r="M60" t="s">
         <v>57</v>
@@ -9944,7 +9944,7 @@
         <v>102</v>
       </c>
       <c r="U72">
-        <v>49.05396767292149</v>
+        <v>49.0539676729215</v>
       </c>
       <c r="V72">
         <v>72.44</v>
@@ -10072,7 +10072,7 @@
         <v>102</v>
       </c>
       <c r="U73">
-        <v>49.05396767292149</v>
+        <v>49.0539676729215</v>
       </c>
       <c r="V73">
         <v>72.44</v>

</xml_diff>